<commit_message>
updating chrome driver test data requires new emails
</commit_message>
<xml_diff>
--- a/src/test/resources/data/LoginData.xlsx
+++ b/src/test/resources/data/LoginData.xlsx
@@ -1,39 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent>
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Eclipse\DDTExample\src\test\resources\data\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr documentId="13_ncr:1_{E2E8D717-6125-4565-9789-F2D705A29A52}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45"/>
+  <xr:revisionPtr documentId="13_ncr:801_{B2DB77B1-0F14-489D-8A27-5A7F1CEC3014}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45"/>
   <bookViews>
-    <workbookView windowHeight="11385" windowWidth="21600" xWindow="5250" xr2:uid="{7DF8A32D-8DD3-47F4-88AD-A1CB416DB106}" yWindow="4215"/>
+    <workbookView windowHeight="16500" windowWidth="21660" xWindow="1170" xr2:uid="{7DF8A32D-8DD3-47F4-88AD-A1CB416DB106}" yWindow="1170"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" r:id="rId1" sheetId="1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
   <extLst>
     <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
   <si>
     <t>Password</t>
   </si>
@@ -50,9 +38,6 @@
     <t>Email</t>
   </si>
   <si>
-    <t>test999@gmail.com</t>
-  </si>
-  <si>
     <t>malik999@gmail.com</t>
   </si>
   <si>
@@ -62,9 +47,6 @@
     <t>Bob999@gmail.com</t>
   </si>
   <si>
-    <t>root root</t>
-  </si>
-  <si>
     <t>Malik Ali</t>
   </si>
   <si>
@@ -86,7 +68,10 @@
     <t>fullname</t>
   </si>
   <si>
-    <t>test</t>
+    <t>mka999@gmail.com</t>
+  </si>
+  <si>
+    <t>mka mka</t>
   </si>
   <si>
     <t>Successful</t>
@@ -459,7 +444,7 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:E5"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -479,10 +464,10 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E1" t="s">
         <v>1</v>
@@ -490,78 +475,60 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="B2" t="s">
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="D2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" t="s">
         <v>18</v>
-      </c>
-      <c r="E2" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E3" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E4" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B5" t="s">
         <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" t="s">
-        <v>18</v>
-      </c>
-      <c r="E5" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="A2" xr:uid="{BD088AB8-2210-41BE-84CD-6F95C2B33CFE}"/>
-    <hyperlink r:id="rId2" ref="A3" xr:uid="{0D845A37-D1E1-48CA-9A92-FFF7416B0351}"/>
-    <hyperlink r:id="rId3" ref="A4" xr:uid="{ED594C2C-2083-4D8F-BEC3-B0A1E14644A9}"/>
-    <hyperlink r:id="rId4" ref="A5" xr:uid="{1A053FC2-879D-494E-A8F3-AC65B7D49607}"/>
+    <hyperlink r:id="rId1" ref="A3" xr:uid="{0D845A37-D1E1-48CA-9A92-FFF7416B0351}"/>
+    <hyperlink r:id="rId2" ref="A4" xr:uid="{ED594C2C-2083-4D8F-BEC3-B0A1E14644A9}"/>
+    <hyperlink r:id="rId3" ref="A5" xr:uid="{1A053FC2-879D-494E-A8F3-AC65B7D49607}"/>
+    <hyperlink r:id="rId4" ref="A2" xr:uid="{47881702-8F0F-49C2-BFEE-19CCBC828729}"/>
   </hyperlinks>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
updating chrome driver 91
</commit_message>
<xml_diff>
--- a/src/test/resources/data/LoginData.xlsx
+++ b/src/test/resources/data/LoginData.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr documentId="13_ncr:801_{B2DB77B1-0F14-489D-8A27-5A7F1CEC3014}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{2A21C1F9-D3BE-4418-8F64-78FCC0724AC1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView windowHeight="16500" windowWidth="21660" xWindow="1170" xr2:uid="{7DF8A32D-8DD3-47F4-88AD-A1CB416DB106}" yWindow="1170"/>
+    <workbookView xWindow="1950" yWindow="1950" windowWidth="21690" windowHeight="16500" xr2:uid="{7DF8A32D-8DD3-47F4-88AD-A1CB416DB106}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" r:id="rId1" sheetId="1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
   <oleSize ref="A1"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Password</t>
   </si>
@@ -72,19 +72,12 @@
   </si>
   <si>
     <t>mka mka</t>
-  </si>
-  <si>
-    <t>Successful</t>
-  </si>
-  <si>
-    <t>Passed</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -120,19 +113,19 @@
     </border>
   </borders>
   <cellStyleXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -149,10 +142,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -187,7 +180,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -239,7 +232,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -350,21 +343,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -381,7 +374,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -433,27 +426,27 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFA1A9BD-24A6-4930-A8BA-F9D46C98F3B2}">
-  <dimension ref="A1:F5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFA1A9BD-24A6-4930-A8BA-F9D46C98F3B2}">
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="D2" sqref="D2:E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="20.140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="10.0" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="9.42578125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="6.42578125" collapsed="true"/>
+    <col min="1" max="1" width="20.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="10" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="6.42578125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -483,12 +476,6 @@
       <c r="C2" t="s">
         <v>16</v>
       </c>
-      <c r="D2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E2" t="s">
-        <v>18</v>
-      </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
@@ -525,11 +512,11 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="A3" xr:uid="{0D845A37-D1E1-48CA-9A92-FFF7416B0351}"/>
-    <hyperlink r:id="rId2" ref="A4" xr:uid="{ED594C2C-2083-4D8F-BEC3-B0A1E14644A9}"/>
-    <hyperlink r:id="rId3" ref="A5" xr:uid="{1A053FC2-879D-494E-A8F3-AC65B7D49607}"/>
-    <hyperlink r:id="rId4" ref="A2" xr:uid="{47881702-8F0F-49C2-BFEE-19CCBC828729}"/>
+    <hyperlink ref="A3" r:id="rId1" xr:uid="{0D845A37-D1E1-48CA-9A92-FFF7416B0351}"/>
+    <hyperlink ref="A4" r:id="rId2" xr:uid="{ED594C2C-2083-4D8F-BEC3-B0A1E14644A9}"/>
+    <hyperlink ref="A5" r:id="rId3" xr:uid="{1A053FC2-879D-494E-A8F3-AC65B7D49607}"/>
+    <hyperlink ref="A2" r:id="rId4" xr:uid="{47881702-8F0F-49C2-BFEE-19CCBC828729}"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>